<commit_message>
plot shear flow cte and steps
</commit_message>
<xml_diff>
--- a/data/10pct_0WSt_and_Car-Thixotropy.xlsx
+++ b/data/10pct_0WSt_and_Car-Thixotropy.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,227 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sample</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>K</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>K err</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>n err</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>sigmaZero</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>sigmaZero err</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>10_0WSt</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>-37.25937124633992</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2.769834849532721</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.2572491832092542</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.01070484742812701</v>
-      </c>
-      <c r="F2" t="n">
-        <v>338.5470087949109</v>
-      </c>
-      <c r="G2" t="n">
-        <v>3.422634039179872</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>10_0WSt</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>-45.48202946472071</v>
-      </c>
-      <c r="C3" t="n">
-        <v>6.32640921675686</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.2806909389601359</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.01851974925124464</v>
-      </c>
-      <c r="F3" t="n">
-        <v>456.0744916721577</v>
-      </c>
-      <c r="G3" t="n">
-        <v>9.042294678478525</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>10_0WSt_iCar</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>-7.439138896617572</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.8925169874153203</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.3650825561207396</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.01564421798854901</v>
-      </c>
-      <c r="F4" t="n">
-        <v>445.2594158827805</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1.884122927256547</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>10_0WSt_iCar</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>-12.6572547518657</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.8497356174801666</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.20864954108277</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.007553550967814023</v>
-      </c>
-      <c r="F5" t="n">
-        <v>464.0058958314584</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1.093367294256617</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>10_0WSt_iCar</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>-7.121161311222956</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2.349629285851734</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.2677602238641908</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.04133612357866206</v>
-      </c>
-      <c r="F6" t="n">
-        <v>518.0433011389191</v>
-      </c>
-      <c r="G6" t="n">
-        <v>3.442910313331477</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>10_0WSt_kCar</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>-164.5681582554509</v>
-      </c>
-      <c r="C7" t="n">
-        <v>3.645853751844414</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.07752969621069035</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.002211238148403796</v>
-      </c>
-      <c r="F7" t="n">
-        <v>404.0117177619999</v>
-      </c>
-      <c r="G7" t="n">
-        <v>3.491151475265841</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>10_0WSt_kCar</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>-130.5920078823785</v>
-      </c>
-      <c r="C8" t="n">
-        <v>3.223794104163151</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0.08099506068133736</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.002479750609751343</v>
-      </c>
-      <c r="F8" t="n">
-        <v>390.4951110272744</v>
-      </c>
-      <c r="G8" t="n">
-        <v>3.098563105642977</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>